<commit_message>
Update with XMLInputFactory2 results
</commit_message>
<xml_diff>
--- a/Java XXE Test Case Results.xlsx
+++ b/Java XXE Test Case Results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="337">
   <si>
     <t>Filename</t>
   </si>
@@ -1397,12 +1397,97 @@
   <si>
     <t>XQJSaxonSafeBindTestCase.java</t>
   </si>
+  <si>
+    <t>XMLInput2UnsafeDefaultTestCase.java</t>
+  </si>
+  <si>
+    <r>
+      <t>org.codehaus.stax2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XMLInputFactory2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>org.codehaus.stax2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XMLInputFactory2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>XMLInput2SafeAccessTestCase.java</t>
+  </si>
+  <si>
+    <t>XMLInput2SafeExternalTestCase.java</t>
+  </si>
+  <si>
+    <t>XMLInput2UnsafeValidationOffTestCase.java</t>
+  </si>
+  <si>
+    <t>XMLInput2UnsafeValidationOnTestCase.java</t>
+  </si>
+  <si>
+    <t>XMLInput2SafeDTDTestCase.java</t>
+  </si>
+  <si>
+    <t>Proves that XMLInputFactory2 is unsafe by default</t>
+  </si>
+  <si>
+    <t>Proves that setting XMLInputFactory2's ACCESS_EXTERNAL_DTD attribute to null makes the XMLStreamReader safe in Java 7u40 and up</t>
+  </si>
+  <si>
+    <t>Proves that setting XMLInputFactory2's IS_SUPPORTING_EXTERNAL_ENTITIES attribute to false makes the XMLStreamReader safe</t>
+  </si>
+  <si>
+    <t>Proves that disabling validation for the XMLInputFactory2 leaves the XMLStreamReader unsafe</t>
+  </si>
+  <si>
+    <t>Proves that enabling validation for the XMLInputFactory2 leaves the XMLStreamReader unsafe</t>
+  </si>
+  <si>
+    <t>Proves that disabling DTD support for the XMLInputFactory2 makes the XMLStreamReader safe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1481,29 +1566,29 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1512,7 +1597,227 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1894,11 +2199,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76893568"/>
-        <c:axId val="76894144"/>
+        <c:axId val="125980032"/>
+        <c:axId val="125980608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76893568"/>
+        <c:axId val="125980032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1934,13 +2239,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76894144"/>
+        <c:crossAx val="125980608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76894144"/>
+        <c:axId val="125980608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1971,7 +2276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76893568"/>
+        <c:crossAx val="125980032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2104,11 +2409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76895872"/>
-        <c:axId val="76896448"/>
+        <c:axId val="125982336"/>
+        <c:axId val="125982912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76895872"/>
+        <c:axId val="125982336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2138,20 +2443,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76896448"/>
+        <c:crossAx val="125982912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76896448"/>
+        <c:axId val="125982912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2176,14 +2480,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76895872"/>
+        <c:crossAx val="125982336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2316,11 +2619,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156254784"/>
-        <c:axId val="156255360"/>
+        <c:axId val="163660352"/>
+        <c:axId val="163660928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156254784"/>
+        <c:axId val="163660352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2350,20 +2653,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156255360"/>
+        <c:crossAx val="163660928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156255360"/>
+        <c:axId val="163660928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2388,14 +2690,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156254784"/>
+        <c:crossAx val="163660352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2528,11 +2829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156257664"/>
-        <c:axId val="156258240"/>
+        <c:axId val="163663232"/>
+        <c:axId val="163663808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156257664"/>
+        <c:axId val="163663232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2568,13 +2869,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156258240"/>
+        <c:crossAx val="163663808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156258240"/>
+        <c:axId val="163663808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2605,7 +2906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156257664"/>
+        <c:crossAx val="163663232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2738,11 +3039,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156260544"/>
-        <c:axId val="156261120"/>
+        <c:axId val="163666112"/>
+        <c:axId val="163666688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156260544"/>
+        <c:axId val="163666112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2778,13 +3079,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156261120"/>
+        <c:crossAx val="163666688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156261120"/>
+        <c:axId val="163666688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2815,7 +3116,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156260544"/>
+        <c:crossAx val="163666112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2948,11 +3249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156640384"/>
-        <c:axId val="156640960"/>
+        <c:axId val="163980416"/>
+        <c:axId val="163980992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156640384"/>
+        <c:axId val="163980416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2988,13 +3289,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156640960"/>
+        <c:crossAx val="163980992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156640960"/>
+        <c:axId val="163980992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3025,7 +3326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156640384"/>
+        <c:crossAx val="163980416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3158,11 +3459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156643264"/>
-        <c:axId val="156643840"/>
+        <c:axId val="163983296"/>
+        <c:axId val="163983872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156643264"/>
+        <c:axId val="163983296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3198,13 +3499,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156643840"/>
+        <c:crossAx val="163983872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156643840"/>
+        <c:axId val="163983872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3235,7 +3536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156643264"/>
+        <c:crossAx val="163983296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3506,12 +3807,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:I84">
-  <autoFilter ref="A1:I84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:I90">
+  <autoFilter ref="A1:I90"/>
   <tableColumns count="9">
     <tableColumn id="8" name="Tests"/>
     <tableColumn id="3" name="XML Parser" totalsRowLabel="Total"/>
-    <tableColumn id="11" name="Test Title" dataDxfId="47"/>
+    <tableColumn id="11" name="Test Title" dataDxfId="69"/>
     <tableColumn id="9" name="Vulnerability"/>
     <tableColumn id="1" name="Filename"/>
     <tableColumn id="5" name="Testing if…"/>
@@ -3532,10 +3833,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="46"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="45"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="44"/>
-    <tableColumn id="9" name="Score" dataDxfId="43"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="68"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="67"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="66"/>
+    <tableColumn id="9" name="Score" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3550,10 +3851,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="42"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="41"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="40"/>
-    <tableColumn id="9" name="Score" dataDxfId="39"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="64"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="63"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="62"/>
+    <tableColumn id="9" name="Score" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3568,10 +3869,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="38"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="37"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="36"/>
-    <tableColumn id="9" name="Score" dataDxfId="35"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="60"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="59"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="58"/>
+    <tableColumn id="9" name="Score" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3586,10 +3887,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="34"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="33"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="32"/>
-    <tableColumn id="9" name="Score" dataDxfId="31"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="56"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="55"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="54"/>
+    <tableColumn id="9" name="Score" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3604,10 +3905,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="30"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="29"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="28"/>
-    <tableColumn id="9" name="Score" dataDxfId="27"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="52"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="51"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="50"/>
+    <tableColumn id="9" name="Score" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3619,15 +3920,15 @@
   <tableColumns count="9">
     <tableColumn id="3" name="XQuery Parser" totalsRowLabel="Total"/>
     <tableColumn id="1" name="True Positive"/>
-    <tableColumn id="5" name="False Negative" dataDxfId="26">
+    <tableColumn id="5" name="False Negative" dataDxfId="48">
       <calculatedColumnFormula>SUM(C1:C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="25"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="24"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="23"/>
-    <tableColumn id="9" name="Score" dataDxfId="22"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="47"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="46"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="45"/>
+    <tableColumn id="9" name="Score" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3638,18 +3939,18 @@
   <autoFilter ref="A2:I5"/>
   <tableColumns count="9">
     <tableColumn id="3" name="XQuery Parser" totalsRowLabel="Total"/>
-    <tableColumn id="1" name="True Positive" dataDxfId="21">
+    <tableColumn id="1" name="True Positive" dataDxfId="43">
       <calculatedColumnFormula>SUM(B1:B2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
-    <tableColumn id="6" name="False Positive" dataDxfId="20">
+    <tableColumn id="6" name="False Positive" dataDxfId="42">
       <calculatedColumnFormula>SUM(E1:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="19"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="18"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="17"/>
-    <tableColumn id="9" name="Score" dataDxfId="16"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="41"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="40"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="39"/>
+    <tableColumn id="9" name="Score" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3960,10 +4261,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5090,10 +5391,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>324</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>140</v>
@@ -5102,7 +5403,7 @@
         <v>115</v>
       </c>
       <c r="E39" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="F39" t="s">
         <v>21</v>
@@ -5114,111 +5415,111 @@
         <v>95</v>
       </c>
       <c r="I39" t="s">
-        <v>73</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>324</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="D40" t="s">
         <v>115</v>
       </c>
       <c r="E40" t="s">
-        <v>274</v>
+        <v>326</v>
       </c>
       <c r="F40" t="s">
         <v>22</v>
       </c>
       <c r="G40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H40" t="s">
         <v>96</v>
       </c>
       <c r="I40" t="s">
-        <v>74</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
         <v>115</v>
       </c>
       <c r="E41" t="s">
-        <v>275</v>
+        <v>327</v>
       </c>
       <c r="F41" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G41" t="s">
         <v>96</v>
       </c>
       <c r="H41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I41" t="s">
-        <v>75</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D42" t="s">
         <v>115</v>
       </c>
       <c r="E42" t="s">
-        <v>276</v>
+        <v>328</v>
       </c>
       <c r="F42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G42" t="s">
         <v>96</v>
       </c>
       <c r="H42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I42" t="s">
-        <v>222</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D43" t="s">
         <v>115</v>
       </c>
       <c r="E43" t="s">
-        <v>277</v>
+        <v>329</v>
       </c>
       <c r="F43" t="s">
         <v>21</v>
@@ -5230,24 +5531,24 @@
         <v>95</v>
       </c>
       <c r="I43" t="s">
-        <v>223</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>109</v>
+        <v>325</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D44" t="s">
         <v>115</v>
       </c>
       <c r="E44" t="s">
-        <v>278</v>
+        <v>330</v>
       </c>
       <c r="F44" t="s">
         <v>22</v>
@@ -5256,85 +5557,85 @@
         <v>96</v>
       </c>
       <c r="H44" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I44" t="s">
-        <v>196</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="D45" t="s">
         <v>115</v>
       </c>
       <c r="E45" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F45" t="s">
         <v>21</v>
       </c>
       <c r="G45" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" t="s">
         <v>95</v>
       </c>
-      <c r="H45" t="s">
-        <v>96</v>
-      </c>
       <c r="I45" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>39</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s">
         <v>115</v>
       </c>
       <c r="E46" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F46" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H46" t="s">
         <v>96</v>
       </c>
       <c r="I46" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>116</v>
+        <v>150</v>
+      </c>
+      <c r="D47" t="s">
+        <v>115</v>
       </c>
       <c r="E47" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F47" t="s">
         <v>21</v>
@@ -5343,30 +5644,30 @@
         <v>96</v>
       </c>
       <c r="H47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I47" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>116</v>
+        <v>155</v>
+      </c>
+      <c r="D48" t="s">
+        <v>115</v>
       </c>
       <c r="E48" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G48" t="s">
         <v>96</v>
@@ -5375,82 +5676,82 @@
         <v>96</v>
       </c>
       <c r="I48" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>116</v>
+        <v>152</v>
+      </c>
+      <c r="D49" t="s">
+        <v>115</v>
       </c>
       <c r="E49" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G49" t="s">
+        <v>96</v>
+      </c>
+      <c r="H49" t="s">
         <v>95</v>
       </c>
-      <c r="H49" t="s">
-        <v>96</v>
-      </c>
       <c r="I49" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>116</v>
+        <v>163</v>
+      </c>
+      <c r="D50" t="s">
+        <v>115</v>
       </c>
       <c r="E50" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F50" t="s">
         <v>22</v>
       </c>
       <c r="G50" t="s">
+        <v>96</v>
+      </c>
+      <c r="H50" t="s">
         <v>95</v>
       </c>
-      <c r="H50" t="s">
-        <v>96</v>
-      </c>
       <c r="I50" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>312</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>116</v>
+        <v>164</v>
+      </c>
+      <c r="D51" t="s">
+        <v>115</v>
       </c>
       <c r="E51" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F51" t="s">
         <v>21</v>
@@ -5459,27 +5760,27 @@
         <v>95</v>
       </c>
       <c r="H51" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I51" t="s">
-        <v>199</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>312</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>116</v>
+        <v>165</v>
+      </c>
+      <c r="D52" t="s">
+        <v>115</v>
       </c>
       <c r="E52" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F52" t="s">
         <v>21</v>
@@ -5488,30 +5789,30 @@
         <v>95</v>
       </c>
       <c r="H52" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I52" t="s">
-        <v>229</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>312</v>
+        <v>119</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E53" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G53" t="s">
         <v>96</v>
@@ -5520,27 +5821,27 @@
         <v>96</v>
       </c>
       <c r="I53" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>312</v>
+        <v>119</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E54" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G54" t="s">
         <v>96</v>
@@ -5549,172 +5850,172 @@
         <v>96</v>
       </c>
       <c r="I54" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>313</v>
+        <v>119</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E55" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F55" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H55" t="s">
         <v>96</v>
       </c>
       <c r="I55" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>313</v>
+        <v>119</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E56" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="F56" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H56" t="s">
         <v>96</v>
       </c>
       <c r="I56" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E57" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I57" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E58" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G58" t="s">
         <v>95</v>
       </c>
       <c r="H58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I58" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E59" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="F59" t="s">
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H59" t="s">
         <v>96</v>
       </c>
       <c r="I59" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E60" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="F60" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G60" t="s">
         <v>96</v>
@@ -5723,24 +6024,24 @@
         <v>96</v>
       </c>
       <c r="I60" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E61" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F61" t="s">
         <v>21</v>
@@ -5752,27 +6053,27 @@
         <v>96</v>
       </c>
       <c r="I61" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E62" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G62" t="s">
         <v>96</v>
@@ -5781,53 +6082,53 @@
         <v>96</v>
       </c>
       <c r="I62" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>217</v>
+        <v>171</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E63" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="F63" t="s">
         <v>22</v>
       </c>
       <c r="G63" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H63" t="s">
         <v>96</v>
       </c>
       <c r="I63" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E64" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F64" t="s">
         <v>22</v>
@@ -5839,111 +6140,111 @@
         <v>96</v>
       </c>
       <c r="I64" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>137</v>
+        <v>313</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E65" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G65" t="s">
         <v>95</v>
       </c>
       <c r="H65" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I65" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>137</v>
+        <v>314</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E66" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F66" t="s">
         <v>21</v>
       </c>
       <c r="G66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I66" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>137</v>
+        <v>314</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E67" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F67" t="s">
         <v>21</v>
       </c>
       <c r="G67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I67" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>137</v>
+        <v>314</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E68" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F68" t="s">
         <v>22</v>
@@ -5955,227 +6256,227 @@
         <v>96</v>
       </c>
       <c r="I68" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>314</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E69" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="F69" t="s">
         <v>22</v>
       </c>
       <c r="G69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H69" t="s">
         <v>96</v>
       </c>
       <c r="I69" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E70" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="F70" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H70" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I70" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>315</v>
+        <v>137</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E71" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F71" t="s">
         <v>21</v>
       </c>
       <c r="G71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H71" t="s">
         <v>95</v>
       </c>
       <c r="I71" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>315</v>
+        <v>137</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E72" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="F72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I72" t="s">
-        <v>129</v>
+        <v>232</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>315</v>
+        <v>137</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E73" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G73" t="s">
         <v>95</v>
       </c>
       <c r="H73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I73" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>315</v>
+        <v>137</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E74" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F74" t="s">
         <v>22</v>
       </c>
       <c r="G74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H74" t="s">
         <v>96</v>
       </c>
       <c r="I74" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>315</v>
+        <v>137</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E75" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F75" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G75" t="s">
         <v>96</v>
       </c>
       <c r="H75" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I75" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E76" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F76" t="s">
         <v>21</v>
@@ -6187,82 +6488,82 @@
         <v>95</v>
       </c>
       <c r="I76" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E77" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="F77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G77" t="s">
         <v>96</v>
       </c>
       <c r="H77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I77" t="s">
-        <v>131</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E78" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="F78" t="s">
         <v>22</v>
       </c>
       <c r="G78" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H78" t="s">
         <v>96</v>
       </c>
       <c r="I78" t="s">
-        <v>227</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E79" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F79" t="s">
         <v>22</v>
@@ -6274,53 +6575,53 @@
         <v>96</v>
       </c>
       <c r="I79" t="s">
-        <v>132</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E80" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="F80" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H80" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I80" t="s">
-        <v>209</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E81" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="F81" t="s">
         <v>21</v>
@@ -6332,82 +6633,82 @@
         <v>95</v>
       </c>
       <c r="I81" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E82" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G82" t="s">
         <v>96</v>
       </c>
       <c r="H82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I82" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E83" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F83" t="s">
         <v>22</v>
       </c>
       <c r="G83" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H83" t="s">
         <v>96</v>
       </c>
       <c r="I83" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E84" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F84" t="s">
         <v>22</v>
@@ -6419,53 +6720,256 @@
         <v>96</v>
       </c>
       <c r="I84" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>78</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E85" t="s">
+        <v>311</v>
+      </c>
+      <c r="F85" t="s">
+        <v>22</v>
+      </c>
+      <c r="G85" t="s">
+        <v>95</v>
+      </c>
+      <c r="H85" t="s">
+        <v>96</v>
+      </c>
+      <c r="I85" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>79</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E86" t="s">
+        <v>316</v>
+      </c>
+      <c r="F86" t="s">
+        <v>21</v>
+      </c>
+      <c r="G86" t="s">
+        <v>96</v>
+      </c>
+      <c r="H86" t="s">
+        <v>95</v>
+      </c>
+      <c r="I86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>80</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E87" t="s">
+        <v>317</v>
+      </c>
+      <c r="F87" t="s">
+        <v>21</v>
+      </c>
+      <c r="G87" t="s">
+        <v>96</v>
+      </c>
+      <c r="H87" t="s">
+        <v>95</v>
+      </c>
+      <c r="I87" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>81</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E88" t="s">
+        <v>320</v>
+      </c>
+      <c r="F88" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" t="s">
+        <v>96</v>
+      </c>
+      <c r="H88" t="s">
+        <v>96</v>
+      </c>
+      <c r="I88" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>82</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E89" t="s">
+        <v>318</v>
+      </c>
+      <c r="F89" t="s">
+        <v>22</v>
+      </c>
+      <c r="G89" t="s">
+        <v>95</v>
+      </c>
+      <c r="H89" t="s">
+        <v>96</v>
+      </c>
+      <c r="I89" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>83</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E90" t="s">
+        <v>319</v>
+      </c>
+      <c r="F90" t="s">
+        <v>22</v>
+      </c>
+      <c r="G90" t="s">
+        <v>95</v>
+      </c>
+      <c r="H90" t="s">
+        <v>96</v>
+      </c>
+      <c r="I90" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D85:D87 D92:D1048576 F1:F79">
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Unsafe (Safe">
+  <conditionalFormatting sqref="D91:D93 D98:D1048576 F1:F38 F45:F85">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Unsafe (Safe">
       <formula>NOT(ISERROR(SEARCH("Unsafe (Safe",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Unsafe">
+    <cfRule type="containsText" dxfId="36" priority="20" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="35" priority="21" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E87 E92:E1048576 G84 H83:H84 G1:H83">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="E91:E93 E98:E1048576 G90 H89:H90 G1:H38 G45:H89">
+    <cfRule type="containsText" dxfId="34" priority="18" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="33" priority="19" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E87 E92:E1048576 G84 H83:H84 G1:H83">
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Fail (Pass">
+  <conditionalFormatting sqref="E91:E93 E98:E1048576 G90 H89:H90 G1:H38 G45:H89">
+    <cfRule type="containsText" dxfId="32" priority="16" operator="containsText" text="Fail (Pass">
       <formula>NOT(ISERROR(SEARCH("Fail (Pass",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F80:F84">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Unsafe (Safe">
-      <formula>NOT(ISERROR(SEARCH("Unsafe (Safe",F80)))</formula>
+  <conditionalFormatting sqref="F86:F90">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Unsafe (Safe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe (Safe",F86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Unsafe">
-      <formula>NOT(ISERROR(SEARCH("Unsafe",F80)))</formula>
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Unsafe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe",F86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Safe">
-      <formula>NOT(ISERROR(SEARCH("Safe",F80)))</formula>
+    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="Safe">
+      <formula>NOT(ISERROR(SEARCH("Safe",F86)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Pass (Fail">
+  <conditionalFormatting sqref="H1:H38 H45:H1048576">
+    <cfRule type="containsText" dxfId="28" priority="12" operator="containsText" text="Pass (Fail">
       <formula>NOT(ISERROR(SEARCH("Pass (Fail",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39:F44">
+    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="Unsafe (Safe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe (Safe",F39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="Unsafe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe",F39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="Safe">
+      <formula>NOT(ISERROR(SEARCH("Safe",F39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39:H44">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",G39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",G39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39:H44">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Fail (Pass">
+      <formula>NOT(ISERROR(SEARCH("Fail (Pass",G39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39:H44">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Pass (Fail">
+      <formula>NOT(ISERROR(SEARCH("Pass (Fail",H39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9567,26 +10071,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Unsafe (Safe">
+    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="Unsafe (Safe">
       <formula>NOT(ISERROR(SEARCH("Unsafe (Safe",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Unsafe">
+    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Fail (Pass">
+    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Fail (Pass">
       <formula>NOT(ISERROR(SEARCH("Fail (Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>